<commit_message>
Sent PCB to fab
</commit_message>
<xml_diff>
--- a/Project Outputs for EpicPlus/EpicPlus_initial_order.xlsx
+++ b/Project Outputs for EpicPlus/EpicPlus_initial_order.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="258">
   <si>
     <t>Comment</t>
   </si>
@@ -749,6 +749,45 @@
   </si>
   <si>
     <t>BRACKET RT ANG MOUNT 4-40 STEEL</t>
+  </si>
+  <si>
+    <t>Next Order</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=511-1465-1-ND</t>
+  </si>
+  <si>
+    <t>511-1465-1-ND</t>
+  </si>
+  <si>
+    <t>TCA1A226M8R</t>
+  </si>
+  <si>
+    <t>CAP TANT 22UF 10V 20% SMD</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=CP-3502-ND</t>
+  </si>
+  <si>
+    <t>CP-3502-ND</t>
+  </si>
+  <si>
+    <t>SP-3501</t>
+  </si>
+  <si>
+    <t>CONN 3.5MM MALE STEREO PLUG</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=67-1945-ND</t>
+  </si>
+  <si>
+    <t>67-1945-ND</t>
+  </si>
+  <si>
+    <t>CLS-PC11A125S01R</t>
+  </si>
+  <si>
+    <t>SWITCH PB ILLUM SPST 3A RED</t>
   </si>
 </sst>
 </file>
@@ -757,7 +796,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1269,7 +1308,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1607,14 +1646,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N92"/>
+  <dimension ref="A1:N98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="3630" ySplit="645" topLeftCell="D67" activePane="topRight"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3630" ySplit="645" topLeftCell="C70" activePane="bottomRight"/>
       <selection activeCell="B25" sqref="B25"/>
       <selection pane="topRight" activeCell="F1" sqref="F1:M1"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="A54:XFD72"/>
-      <selection pane="bottomRight" activeCell="M92" sqref="F73:M92"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95"/>
+      <selection pane="bottomRight" activeCell="M96" sqref="F96:M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3207,14 +3246,14 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="K80">
-        <f>$B$25*C80*2</f>
+        <f t="shared" ref="K80:K88" si="13">$B$25*C80*2</f>
         <v>20</v>
       </c>
       <c r="L80" s="3" t="s">
         <v>127</v>
       </c>
       <c r="M80" s="5">
-        <f>K80*J80</f>
+        <f t="shared" ref="M80:M88" si="14">K80*J80</f>
         <v>1.98</v>
       </c>
     </row>
@@ -3241,14 +3280,14 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K81">
-        <f>$B$25*C81*2</f>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>127</v>
       </c>
       <c r="M81" s="5">
-        <f>K81*J81</f>
+        <f t="shared" si="14"/>
         <v>4.5</v>
       </c>
     </row>
@@ -3275,12 +3314,12 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="K82">
-        <f>$B$25*C82*2</f>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
       <c r="L82" s="3"/>
       <c r="M82" s="5">
-        <f>K82*J82</f>
+        <f t="shared" si="14"/>
         <v>11.6</v>
       </c>
     </row>
@@ -3307,14 +3346,14 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="K83">
-        <f>$B$25*C83*2</f>
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
       <c r="L83" s="3" t="s">
         <v>127</v>
       </c>
       <c r="M83" s="5">
-        <f>K83*J83</f>
+        <f t="shared" si="14"/>
         <v>1.46</v>
       </c>
     </row>
@@ -3341,11 +3380,11 @@
         <v>0.01</v>
       </c>
       <c r="K84">
-        <f>$B$25*C84*2</f>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="M84" s="5">
-        <f>K84*J84</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
@@ -3372,14 +3411,14 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="K85">
-        <f>$B$25*C85*2</f>
+        <f t="shared" si="13"/>
         <v>30</v>
       </c>
       <c r="L85" s="3" t="s">
         <v>127</v>
       </c>
       <c r="M85" s="5">
-        <f>K85*J85</f>
+        <f t="shared" si="14"/>
         <v>2.19</v>
       </c>
     </row>
@@ -3406,11 +3445,11 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="K86">
-        <f>$B$25*C86*2</f>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="M86" s="5">
-        <f>K86*J86</f>
+        <f t="shared" si="14"/>
         <v>3.65</v>
       </c>
     </row>
@@ -3437,12 +3476,12 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="K87">
-        <f>$B$25*C87*2</f>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="L87" s="3"/>
       <c r="M87" s="5">
-        <f>K87*J87</f>
+        <f t="shared" si="14"/>
         <v>3.65</v>
       </c>
     </row>
@@ -3469,11 +3508,11 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="K88">
-        <f>$B$25*C88*2</f>
+        <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="M88" s="5">
-        <f>K88*J88</f>
+        <f t="shared" si="14"/>
         <v>3.65</v>
       </c>
     </row>
@@ -3503,7 +3542,7 @@
         <v>5</v>
       </c>
       <c r="M90" s="5">
-        <f t="shared" ref="M90:M92" si="13">K90*J90</f>
+        <f t="shared" ref="M90:M92" si="15">K90*J90</f>
         <v>53.25</v>
       </c>
     </row>
@@ -3527,7 +3566,7 @@
         <v>5</v>
       </c>
       <c r="M91" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>25</v>
       </c>
     </row>
@@ -3551,8 +3590,89 @@
         <v>40</v>
       </c>
       <c r="M92" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>11.200000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="J96" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="K96">
+        <f t="shared" ref="K96" si="16">$B$25*C96*2</f>
+        <v>20</v>
+      </c>
+      <c r="M96" s="5">
+        <f t="shared" ref="M96:M98" si="17">K96*J96</f>
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="97" spans="6:13">
+      <c r="F97" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="J97" s="5">
+        <v>1.04</v>
+      </c>
+      <c r="K97">
+        <v>15</v>
+      </c>
+      <c r="M97" s="5">
+        <f t="shared" si="17"/>
+        <v>15.600000000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="6:13">
+      <c r="F98" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="J98" s="5">
+        <v>3.21</v>
+      </c>
+      <c r="K98">
+        <v>5</v>
+      </c>
+      <c r="M98" s="5">
+        <f t="shared" si="17"/>
+        <v>16.05</v>
       </c>
     </row>
   </sheetData>
@@ -3610,8 +3730,11 @@
     <hyperlink ref="F87" r:id="rId51"/>
     <hyperlink ref="F88" r:id="rId52"/>
     <hyperlink ref="F92" r:id="rId53"/>
+    <hyperlink ref="F96" r:id="rId54"/>
+    <hyperlink ref="F97" r:id="rId55"/>
+    <hyperlink ref="F98" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId54"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>